<commit_message>
to do list overhaul
</commit_message>
<xml_diff>
--- a/To-Do List.xlsx
+++ b/To-Do List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshu\Documents\GitHub\Collab2.gmx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Videos\epic website\Collab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDE648B-D8C5-4715-9A3B-D177694551D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>TASK</t>
   </si>
@@ -42,9 +41,6 @@
     <t>working menus</t>
   </si>
   <si>
-    <t>levels game mode</t>
-  </si>
-  <si>
     <t>better graphics</t>
   </si>
   <si>
@@ -100,12 +96,45 @@
   </si>
   <si>
     <t>Pause Menu</t>
+  </si>
+  <si>
+    <t>Completed?</t>
+  </si>
+  <si>
+    <t>Date completed</t>
+  </si>
+  <si>
+    <t>Later to Do Tasks</t>
+  </si>
+  <si>
+    <t>advanced room animations</t>
+  </si>
+  <si>
+    <t>advanced graphics work</t>
+  </si>
+  <si>
+    <t>intro video</t>
+  </si>
+  <si>
+    <t>end screen transition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single player campaign </t>
+  </si>
+  <si>
+    <t>trailer</t>
+  </si>
+  <si>
+    <t>options menu</t>
+  </si>
+  <si>
+    <t>signatures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -241,6 +276,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,11 +562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8">
         <v>43355</v>
@@ -561,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="7"/>
     </row>
@@ -570,74 +612,80 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43356</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43356</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="8">
         <v>43346</v>
@@ -645,28 +693,26 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C16" s="8">
         <v>43345</v>
@@ -674,10 +720,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8">
         <v>43345</v>
@@ -685,10 +731,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="8">
         <v>43346</v>
@@ -696,10 +742,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="8">
         <v>43346</v>
@@ -707,17 +753,107 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="10"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>